<commit_message>
Justering skript, slette de som erunødvendig
</commit_message>
<xml_diff>
--- a/resultat_antall.xlsx
+++ b/resultat_antall.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -380,15 +380,25 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>tilfeller_mean</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>tilfeller_max</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>død_sum</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>død_mean</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>død_max</t>
         </is>
@@ -398,10 +408,8 @@
       <c r="A2">
         <v>2019</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>desember</t>
-        </is>
+      <c r="B2">
+        <v>12</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -418,6 +426,12 @@
         <v>0</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>0</v>
       </c>
     </row>
@@ -425,10 +439,8 @@
       <c r="A3">
         <v>2019</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>desember</t>
-        </is>
+      <c r="B3">
+        <v>12</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -445,6 +457,12 @@
         <v>0</v>
       </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
     </row>
@@ -452,10 +470,8 @@
       <c r="A4">
         <v>2019</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>desember</t>
-        </is>
+      <c r="B4">
+        <v>12</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -466,12 +482,18 @@
         <v>27</v>
       </c>
       <c r="E4">
+        <v>1.08</v>
+      </c>
+      <c r="F4">
         <v>27</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>0</v>
       </c>
     </row>
@@ -479,10 +501,8 @@
       <c r="A5">
         <v>2019</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>desember</t>
-        </is>
+      <c r="B5">
+        <v>12</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -499,6 +519,12 @@
         <v>0</v>
       </c>
       <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>0</v>
       </c>
     </row>
@@ -506,10 +532,8 @@
       <c r="A6">
         <v>2019</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>desember</t>
-        </is>
+      <c r="B6">
+        <v>12</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -526,6 +550,12 @@
         <v>0</v>
       </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>0</v>
       </c>
     </row>
@@ -533,10 +563,8 @@
       <c r="A7">
         <v>2019</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>desember</t>
-        </is>
+      <c r="B7">
+        <v>12</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -553,6 +581,12 @@
         <v>0</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>0</v>
       </c>
     </row>
@@ -560,10 +594,8 @@
       <c r="A8">
         <v>2020</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>april</t>
-        </is>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -571,26 +603,30 @@
         </is>
       </c>
       <c r="D8">
-        <v>31598</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>463</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>1425</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
         <v>2020</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>april</t>
-        </is>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -598,26 +634,30 @@
         </is>
       </c>
       <c r="D9">
-        <v>1104862</v>
+        <v>9</v>
       </c>
       <c r="E9">
-        <v>48529</v>
+        <v>0.04838709677419355</v>
       </c>
       <c r="F9">
-        <v>70904</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>4928</v>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
         <v>2020</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>april</t>
-        </is>
+      <c r="B10">
+        <v>1</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -625,26 +665,30 @@
         </is>
       </c>
       <c r="D10">
-        <v>333821</v>
+        <v>9766</v>
       </c>
       <c r="E10">
-        <v>5275</v>
+        <v>12.60129032258065</v>
       </c>
       <c r="F10">
-        <v>11321</v>
+        <v>1980</v>
       </c>
       <c r="G10">
-        <v>1290</v>
+        <v>213</v>
+      </c>
+      <c r="H10">
+        <v>0.2748387096774194</v>
+      </c>
+      <c r="I10">
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
         <v>2020</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>april</t>
-        </is>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -652,26 +696,30 @@
         </is>
       </c>
       <c r="D11">
-        <v>857418</v>
+        <v>15</v>
       </c>
       <c r="E11">
-        <v>7583</v>
+        <v>0.01612903225806452</v>
       </c>
       <c r="F11">
-        <v>105393</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>2004</v>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
         <v>2020</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>april</t>
-        </is>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -679,177 +727,207 @@
         </is>
       </c>
       <c r="D12">
-        <v>2812</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>324</v>
+        <v>0.1129032258064516</v>
       </c>
       <c r="F12">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
         <v>2020</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>august</t>
-        </is>
+      <c r="B13">
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D13">
-        <v>336450</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>11014</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>10274</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>414</v>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
         <v>2020</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>august</t>
-        </is>
+      <c r="B14">
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>America</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="D14">
-        <v>4058338</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>67023</v>
+        <v>0.03448275862068966</v>
       </c>
       <c r="F14">
-        <v>112185</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>3935</v>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
         <v>2020</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>august</t>
-        </is>
+      <c r="B15">
+        <v>2</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>America</t>
         </is>
       </c>
       <c r="D15">
-        <v>2799266</v>
+        <v>76</v>
       </c>
       <c r="E15">
-        <v>78761</v>
+        <v>0.4367816091954023</v>
       </c>
       <c r="F15">
-        <v>45643</v>
+        <v>19</v>
       </c>
       <c r="G15">
-        <v>1092</v>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
         <v>2020</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>august</t>
-        </is>
+      <c r="B16">
+        <v>2</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D16">
-        <v>772079</v>
+        <v>73470</v>
       </c>
       <c r="E16">
-        <v>23572</v>
+        <v>101.3379310344828</v>
       </c>
       <c r="F16">
-        <v>10088</v>
+        <v>15141</v>
       </c>
       <c r="G16">
-        <v>181</v>
+        <v>2679</v>
+      </c>
+      <c r="H16">
+        <v>3.695172413793103</v>
+      </c>
+      <c r="I16">
+        <v>254</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
         <v>2020</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>august</t>
-        </is>
+      <c r="B17">
+        <v>2</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="D17">
-        <v>11296</v>
+        <v>1139</v>
       </c>
       <c r="E17">
-        <v>715</v>
+        <v>1.309195402298851</v>
       </c>
       <c r="F17">
-        <v>432</v>
+        <v>250</v>
       </c>
       <c r="G17">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="H17">
+        <v>0.0264367816091954</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
         <v>2020</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>februar</t>
-        </is>
+      <c r="B18">
+        <v>2</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.3275862068965517</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>0</v>
       </c>
     </row>
@@ -857,728 +935,836 @@
       <c r="A19">
         <v>2020</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>februar</t>
-        </is>
+      <c r="B19">
+        <v>2</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>America</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D19">
-        <v>76</v>
+        <v>705</v>
       </c>
       <c r="E19">
-        <v>19</v>
+        <v>24.31034482758621</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>0.2068965517241379</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
         <v>2020</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>februar</t>
-        </is>
+      <c r="B20">
+        <v>3</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="D20">
-        <v>73470</v>
+        <v>5134</v>
       </c>
       <c r="E20">
-        <v>15141</v>
+        <v>7.100968188105117</v>
       </c>
       <c r="F20">
-        <v>2679</v>
+        <v>243</v>
       </c>
       <c r="G20">
-        <v>254</v>
+        <v>166</v>
+      </c>
+      <c r="H20">
+        <v>0.2295988934993084</v>
+      </c>
+      <c r="I20">
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
         <v>2020</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>februar</t>
-        </is>
+      <c r="B21">
+        <v>3</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>America</t>
         </is>
       </c>
       <c r="D21">
-        <v>1139</v>
+        <v>188660</v>
       </c>
       <c r="E21">
-        <v>250</v>
+        <v>257.7322404371585</v>
       </c>
       <c r="F21">
-        <v>23</v>
+        <v>21595</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>3687</v>
+      </c>
+      <c r="H21">
+        <v>5.036885245901639</v>
+      </c>
+      <c r="I21">
+        <v>661</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
         <v>2020</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>februar</t>
-        </is>
+      <c r="B22">
+        <v>3</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D22">
-        <v>19</v>
+        <v>85871</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>91.54690831556503</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>3186</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>3990</v>
+      </c>
+      <c r="H22">
+        <v>4.253731343283582</v>
+      </c>
+      <c r="I22">
+        <v>157</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
         <v>2020</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>februar</t>
-        </is>
+      <c r="B23">
+        <v>3</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="D23">
-        <v>705</v>
+        <v>437423</v>
       </c>
       <c r="E23">
-        <v>134</v>
+        <v>327.6576779026217</v>
       </c>
       <c r="F23">
-        <v>6</v>
+        <v>9181</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>27889</v>
+      </c>
+      <c r="H23">
+        <v>20.89063670411985</v>
+      </c>
+      <c r="I23">
+        <v>971</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
         <v>2020</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>januar</t>
-        </is>
+      <c r="B24">
+        <v>3</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>5298</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>46.47368421052632</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>611</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="H24">
+        <v>0.1842105263157895</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
         <v>2020</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>januar</t>
-        </is>
+      <c r="B25">
+        <v>3</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>America</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="D25">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
         <v>2020</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>januar</t>
-        </is>
+      <c r="B26">
+        <v>4</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="D26">
-        <v>9766</v>
+        <v>31598</v>
       </c>
       <c r="E26">
-        <v>1980</v>
+        <v>20.3858064516129</v>
       </c>
       <c r="F26">
-        <v>213</v>
+        <v>463</v>
       </c>
       <c r="G26">
-        <v>43</v>
+        <v>1425</v>
+      </c>
+      <c r="H26">
+        <v>0.9193548387096774</v>
+      </c>
+      <c r="I26">
+        <v>42</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
         <v>2020</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>januar</t>
-        </is>
+      <c r="B27">
+        <v>4</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>America</t>
         </is>
       </c>
       <c r="D27">
-        <v>15</v>
+        <v>1104862</v>
       </c>
       <c r="E27">
-        <v>3</v>
+        <v>754.1720136518771</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>48529</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>70904</v>
+      </c>
+      <c r="H27">
+        <v>48.39863481228669</v>
+      </c>
+      <c r="I27">
+        <v>4928</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
         <v>2020</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>januar</t>
-        </is>
+      <c r="B28">
+        <v>4</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D28">
-        <v>7</v>
+        <v>333821</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>267.0568</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>5275</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>11321</v>
+      </c>
+      <c r="H28">
+        <v>9.056800000000001</v>
+      </c>
+      <c r="I28">
+        <v>1290</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
         <v>2020</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>januar</t>
-        </is>
+      <c r="B29">
+        <v>4</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>857418</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>529.2703703703704</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>7583</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>105393</v>
+      </c>
+      <c r="H29">
+        <v>65.05740740740741</v>
+      </c>
+      <c r="I29">
+        <v>2004</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
         <v>2020</v>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>juli</t>
-        </is>
+      <c r="B30">
+        <v>4</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="D30">
-        <v>516291</v>
+        <v>2812</v>
       </c>
       <c r="E30">
-        <v>13944</v>
+        <v>11.71666666666667</v>
       </c>
       <c r="F30">
-        <v>9433</v>
+        <v>324</v>
       </c>
       <c r="G30">
-        <v>572</v>
+        <v>95</v>
+      </c>
+      <c r="H30">
+        <v>0.3958333333333333</v>
+      </c>
+      <c r="I30">
+        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
         <v>2020</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>juli</t>
-        </is>
+      <c r="B31">
+        <v>5</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>America</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="D31">
-        <v>4112251</v>
+        <v>104887</v>
       </c>
       <c r="E31">
-        <v>78427</v>
+        <v>62.06331360946746</v>
       </c>
       <c r="F31">
-        <v>106910</v>
+        <v>1837</v>
       </c>
       <c r="G31">
-        <v>3887</v>
+        <v>2480</v>
+      </c>
+      <c r="H31">
+        <v>1.467455621301775</v>
+      </c>
+      <c r="I31">
+        <v>52</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
         <v>2020</v>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>juli</t>
-        </is>
+      <c r="B32">
+        <v>5</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>America</t>
         </is>
       </c>
       <c r="D32">
-        <v>1929728</v>
+        <v>1552784</v>
       </c>
       <c r="E32">
-        <v>55078</v>
+        <v>1022.2409479921</v>
       </c>
       <c r="F32">
-        <v>39033</v>
+        <v>33955</v>
       </c>
       <c r="G32">
-        <v>1129</v>
+        <v>86923</v>
+      </c>
+      <c r="H32">
+        <v>57.2238314680711</v>
+      </c>
+      <c r="I32">
+        <v>2353</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
         <v>2020</v>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>juli</t>
-        </is>
+      <c r="B33">
+        <v>5</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D33">
-        <v>486131</v>
+        <v>592831</v>
       </c>
       <c r="E33">
-        <v>6760</v>
+        <v>444.7344336084021</v>
       </c>
       <c r="F33">
-        <v>10758</v>
+        <v>8380</v>
       </c>
       <c r="G33">
-        <v>216</v>
+        <v>11862</v>
+      </c>
+      <c r="H33">
+        <v>8.898724681170293</v>
+      </c>
+      <c r="I33">
+        <v>265</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
         <v>2020</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>juli</t>
-        </is>
+      <c r="B34">
+        <v>5</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="D34">
-        <v>8750</v>
+        <v>623096</v>
       </c>
       <c r="E34">
-        <v>721</v>
+        <v>372.2198327359618</v>
       </c>
       <c r="F34">
-        <v>87</v>
+        <v>11656</v>
       </c>
       <c r="G34">
-        <v>13</v>
+        <v>38913</v>
+      </c>
+      <c r="H34">
+        <v>23.24551971326165</v>
+      </c>
+      <c r="I34">
+        <v>726</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
         <v>2020</v>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>juni</t>
-        </is>
+      <c r="B35">
+        <v>5</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="D35">
-        <v>251822</v>
+        <v>503</v>
       </c>
       <c r="E35">
-        <v>7210</v>
+        <v>2.028225806451613</v>
       </c>
       <c r="F35">
-        <v>5807</v>
+        <v>30</v>
       </c>
       <c r="G35">
-        <v>111</v>
+        <v>15</v>
+      </c>
+      <c r="H35">
+        <v>0.06048387096774194</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
         <v>2020</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>juni</t>
-        </is>
+      <c r="B36">
+        <v>6</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>America</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="D36">
-        <v>2379672</v>
+        <v>251822</v>
       </c>
       <c r="E36">
-        <v>54771</v>
+        <v>152.6193939393939</v>
       </c>
       <c r="F36">
-        <v>87158</v>
+        <v>7210</v>
       </c>
       <c r="G36">
-        <v>2437</v>
+        <v>5807</v>
+      </c>
+      <c r="H36">
+        <v>3.51939393939394</v>
+      </c>
+      <c r="I36">
+        <v>111</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
         <v>2020</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>juni</t>
-        </is>
+      <c r="B37">
+        <v>6</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>America</t>
         </is>
       </c>
       <c r="D37">
-        <v>1119998</v>
+        <v>2379672</v>
       </c>
       <c r="E37">
-        <v>19906</v>
+        <v>1619.926480599047</v>
       </c>
       <c r="F37">
-        <v>25129</v>
+        <v>54771</v>
       </c>
       <c r="G37">
-        <v>2003</v>
+        <v>87158</v>
+      </c>
+      <c r="H37">
+        <v>59.33151803948264</v>
+      </c>
+      <c r="I37">
+        <v>2437</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
         <v>2020</v>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>juni</t>
-        </is>
+      <c r="B38">
+        <v>6</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D38">
-        <v>480790</v>
+        <v>1119998</v>
       </c>
       <c r="E38">
-        <v>9268</v>
+        <v>868.215503875969</v>
       </c>
       <c r="F38">
-        <v>16003</v>
+        <v>19906</v>
       </c>
       <c r="G38">
-        <v>1179</v>
+        <v>25129</v>
+      </c>
+      <c r="H38">
+        <v>19.47984496124031</v>
+      </c>
+      <c r="I38">
+        <v>2003</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
         <v>2020</v>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>juni</t>
-        </is>
+      <c r="B39">
+        <v>6</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="D39">
-        <v>705</v>
+        <v>480790</v>
       </c>
       <c r="E39">
-        <v>81</v>
+        <v>296.783950617284</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>9268</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>16003</v>
+      </c>
+      <c r="H39">
+        <v>9.878395061728394</v>
+      </c>
+      <c r="I39">
+        <v>1179</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
         <v>2020</v>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>mai</t>
-        </is>
+      <c r="B40">
+        <v>6</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="D40">
-        <v>104887</v>
+        <v>705</v>
       </c>
       <c r="E40">
-        <v>1837</v>
+        <v>2.9375</v>
       </c>
       <c r="F40">
-        <v>2480</v>
+        <v>81</v>
       </c>
       <c r="G40">
-        <v>52</v>
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>0.008333333333333333</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
         <v>2020</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>mai</t>
-        </is>
+      <c r="B41">
+        <v>7</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>America</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="D41">
-        <v>1552784</v>
+        <v>516291</v>
       </c>
       <c r="E41">
-        <v>33955</v>
+        <v>302.8099706744868</v>
       </c>
       <c r="F41">
-        <v>86923</v>
+        <v>13944</v>
       </c>
       <c r="G41">
-        <v>2353</v>
+        <v>9433</v>
+      </c>
+      <c r="H41">
+        <v>5.532551319648094</v>
+      </c>
+      <c r="I41">
+        <v>572</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
         <v>2020</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>mai</t>
-        </is>
+      <c r="B42">
+        <v>7</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>America</t>
         </is>
       </c>
       <c r="D42">
-        <v>592831</v>
+        <v>4112251</v>
       </c>
       <c r="E42">
-        <v>8380</v>
+        <v>2707.209348255431</v>
       </c>
       <c r="F42">
-        <v>11862</v>
+        <v>78427</v>
       </c>
       <c r="G42">
-        <v>265</v>
+        <v>106910</v>
+      </c>
+      <c r="H42">
+        <v>70.3818301514154</v>
+      </c>
+      <c r="I42">
+        <v>3887</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
         <v>2020</v>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>mai</t>
-        </is>
+      <c r="B43">
+        <v>7</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D43">
-        <v>623096</v>
+        <v>1929728</v>
       </c>
       <c r="E43">
-        <v>11656</v>
+        <v>1447.65791447862</v>
       </c>
       <c r="F43">
-        <v>38913</v>
+        <v>55078</v>
       </c>
       <c r="G43">
-        <v>726</v>
+        <v>39033</v>
+      </c>
+      <c r="H43">
+        <v>29.28207051762941</v>
+      </c>
+      <c r="I43">
+        <v>1129</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
         <v>2020</v>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>mai</t>
-        </is>
+      <c r="B44">
+        <v>7</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="D44">
-        <v>503</v>
+        <v>486131</v>
       </c>
       <c r="E44">
-        <v>30</v>
+        <v>290.4008363201912</v>
       </c>
       <c r="F44">
-        <v>15</v>
+        <v>6760</v>
       </c>
       <c r="G44">
-        <v>2</v>
+        <v>10758</v>
+      </c>
+      <c r="H44">
+        <v>6.426523297491039</v>
+      </c>
+      <c r="I44">
+        <v>216</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
         <v>2020</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>mars</t>
-        </is>
+      <c r="B45">
+        <v>7</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="D45">
-        <v>5134</v>
+        <v>8750</v>
       </c>
       <c r="E45">
-        <v>243</v>
+        <v>35.28225806451613</v>
       </c>
       <c r="F45">
-        <v>166</v>
+        <v>721</v>
       </c>
       <c r="G45">
+        <v>87</v>
+      </c>
+      <c r="H45">
+        <v>0.3508064516129033</v>
+      </c>
+      <c r="I45">
         <v>13</v>
       </c>
     </row>
@@ -1586,145 +1772,163 @@
       <c r="A46">
         <v>2020</v>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>mars</t>
-        </is>
+      <c r="B46">
+        <v>8</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>America</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="D46">
-        <v>188660</v>
+        <v>336450</v>
       </c>
       <c r="E46">
-        <v>21595</v>
+        <v>197.3313782991203</v>
       </c>
       <c r="F46">
-        <v>3687</v>
+        <v>11014</v>
       </c>
       <c r="G46">
-        <v>661</v>
+        <v>10274</v>
+      </c>
+      <c r="H46">
+        <v>6.025806451612903</v>
+      </c>
+      <c r="I46">
+        <v>414</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
         <v>2020</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>mars</t>
-        </is>
+      <c r="B47">
+        <v>8</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>America</t>
         </is>
       </c>
       <c r="D47">
-        <v>85871</v>
+        <v>4058338</v>
       </c>
       <c r="E47">
-        <v>3186</v>
+        <v>2671.716919025675</v>
       </c>
       <c r="F47">
-        <v>3990</v>
+        <v>67023</v>
       </c>
       <c r="G47">
-        <v>157</v>
+        <v>112185</v>
+      </c>
+      <c r="H47">
+        <v>73.85450954575379</v>
+      </c>
+      <c r="I47">
+        <v>3935</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
         <v>2020</v>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>mars</t>
-        </is>
+      <c r="B48">
+        <v>8</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D48">
-        <v>437423</v>
+        <v>2799266</v>
       </c>
       <c r="E48">
-        <v>9181</v>
+        <v>2099.974493623406</v>
       </c>
       <c r="F48">
-        <v>27889</v>
+        <v>78761</v>
       </c>
       <c r="G48">
-        <v>971</v>
+        <v>45643</v>
+      </c>
+      <c r="H48">
+        <v>34.24081020255064</v>
+      </c>
+      <c r="I48">
+        <v>1092</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
         <v>2020</v>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>mars</t>
-        </is>
+      <c r="B49">
+        <v>8</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="D49">
-        <v>5298</v>
+        <v>772079</v>
       </c>
       <c r="E49">
-        <v>611</v>
+        <v>461.2180406212664</v>
       </c>
       <c r="F49">
-        <v>21</v>
+        <v>23572</v>
       </c>
       <c r="G49">
-        <v>3</v>
+        <v>10088</v>
+      </c>
+      <c r="H49">
+        <v>6.026284348864994</v>
+      </c>
+      <c r="I49">
+        <v>181</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
         <v>2020</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>mars</t>
-        </is>
+      <c r="B50">
+        <v>8</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="D50">
-        <v>-9</v>
+        <v>11296</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>45.54838709677419</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>715</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>432</v>
+      </c>
+      <c r="H50">
+        <v>1.741935483870968</v>
+      </c>
+      <c r="I50">
+        <v>25</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
         <v>2020</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>oktober</t>
-        </is>
+      <c r="B51">
+        <v>9</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1732,26 +1936,30 @@
         </is>
       </c>
       <c r="D51">
-        <v>131812</v>
+        <v>228136</v>
       </c>
       <c r="E51">
-        <v>3920</v>
+        <v>138.2642424242424</v>
       </c>
       <c r="F51">
-        <v>3157</v>
+        <v>4305</v>
       </c>
       <c r="G51">
-        <v>248</v>
+        <v>6088</v>
+      </c>
+      <c r="H51">
+        <v>3.68969696969697</v>
+      </c>
+      <c r="I51">
+        <v>188</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
         <v>2020</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>oktober</t>
-        </is>
+      <c r="B52">
+        <v>9</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1759,26 +1967,30 @@
         </is>
       </c>
       <c r="D52">
-        <v>1691893</v>
+        <v>3282395</v>
       </c>
       <c r="E52">
-        <v>59386</v>
+        <v>2232.921768707483</v>
       </c>
       <c r="F52">
-        <v>43473</v>
+        <v>55013</v>
       </c>
       <c r="G52">
-        <v>3351</v>
+        <v>89303</v>
+      </c>
+      <c r="H52">
+        <v>60.75034013605442</v>
+      </c>
+      <c r="I52">
+        <v>3800</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
         <v>2020</v>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>oktober</t>
-        </is>
+      <c r="B53">
+        <v>9</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1786,26 +1998,30 @@
         </is>
       </c>
       <c r="D53">
-        <v>1601844</v>
+        <v>3512145</v>
       </c>
       <c r="E53">
-        <v>86821</v>
+        <v>2722.593023255814</v>
       </c>
       <c r="F53">
-        <v>24633</v>
+        <v>97894</v>
       </c>
       <c r="G53">
-        <v>1181</v>
+        <v>51806</v>
+      </c>
+      <c r="H53">
+        <v>40.15968992248062</v>
+      </c>
+      <c r="I53">
+        <v>1290</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
         <v>2020</v>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>oktober</t>
-        </is>
+      <c r="B54">
+        <v>9</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1813,26 +2029,30 @@
         </is>
       </c>
       <c r="D54">
-        <v>1420856</v>
+        <v>1429324</v>
       </c>
       <c r="E54">
-        <v>27856</v>
+        <v>882.2987654320988</v>
       </c>
       <c r="F54">
-        <v>12717</v>
+        <v>31785</v>
       </c>
       <c r="G54">
-        <v>261</v>
+        <v>14653</v>
+      </c>
+      <c r="H54">
+        <v>9.045061728395062</v>
+      </c>
+      <c r="I54">
+        <v>241</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
         <v>2020</v>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>oktober</t>
-        </is>
+      <c r="B55">
+        <v>9</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1840,26 +2060,30 @@
         </is>
       </c>
       <c r="D55">
-        <v>3112</v>
+        <v>3925</v>
       </c>
       <c r="E55">
-        <v>497</v>
+        <v>16.35416666666667</v>
       </c>
       <c r="F55">
-        <v>42</v>
+        <v>334</v>
       </c>
       <c r="G55">
-        <v>6</v>
+        <v>320</v>
+      </c>
+      <c r="H55">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="I55">
+        <v>59</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
         <v>2020</v>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>september</t>
-        </is>
+      <c r="B56">
+        <v>10</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1867,26 +2091,30 @@
         </is>
       </c>
       <c r="D56">
-        <v>228136</v>
+        <v>131812</v>
       </c>
       <c r="E56">
-        <v>4305</v>
+        <v>159.7721212121212</v>
       </c>
       <c r="F56">
-        <v>6088</v>
+        <v>3920</v>
       </c>
       <c r="G56">
-        <v>188</v>
+        <v>3157</v>
+      </c>
+      <c r="H56">
+        <v>3.826666666666667</v>
+      </c>
+      <c r="I56">
+        <v>248</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
         <v>2020</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>september</t>
-        </is>
+      <c r="B57">
+        <v>10</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1894,26 +2122,30 @@
         </is>
       </c>
       <c r="D57">
-        <v>3282395</v>
+        <v>1691893</v>
       </c>
       <c r="E57">
-        <v>55013</v>
+        <v>2301.895238095238</v>
       </c>
       <c r="F57">
-        <v>89303</v>
+        <v>59386</v>
       </c>
       <c r="G57">
-        <v>3800</v>
+        <v>43473</v>
+      </c>
+      <c r="H57">
+        <v>59.14693877551021</v>
+      </c>
+      <c r="I57">
+        <v>3351</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
         <v>2020</v>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>september</t>
-        </is>
+      <c r="B58">
+        <v>10</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1921,26 +2153,30 @@
         </is>
       </c>
       <c r="D58">
-        <v>3512145</v>
+        <v>1601844</v>
       </c>
       <c r="E58">
-        <v>97894</v>
+        <v>2483.479069767442</v>
       </c>
       <c r="F58">
-        <v>51806</v>
+        <v>86821</v>
       </c>
       <c r="G58">
-        <v>1290</v>
+        <v>24633</v>
+      </c>
+      <c r="H58">
+        <v>38.19069767441861</v>
+      </c>
+      <c r="I58">
+        <v>1181</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
         <v>2020</v>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>september</t>
-        </is>
+      <c r="B59">
+        <v>10</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1948,26 +2184,30 @@
         </is>
       </c>
       <c r="D59">
-        <v>1429324</v>
+        <v>1420856</v>
       </c>
       <c r="E59">
-        <v>31785</v>
+        <v>1756.311495673671</v>
       </c>
       <c r="F59">
-        <v>14653</v>
+        <v>27856</v>
       </c>
       <c r="G59">
-        <v>241</v>
+        <v>12717</v>
+      </c>
+      <c r="H59">
+        <v>15.71940667490729</v>
+      </c>
+      <c r="I59">
+        <v>261</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
         <v>2020</v>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>september</t>
-        </is>
+      <c r="B60">
+        <v>10</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1975,16 +2215,22 @@
         </is>
       </c>
       <c r="D60">
-        <v>3925</v>
+        <v>3112</v>
       </c>
       <c r="E60">
-        <v>334</v>
+        <v>25.93333333333333</v>
       </c>
       <c r="F60">
-        <v>320</v>
+        <v>497</v>
       </c>
       <c r="G60">
-        <v>59</v>
+        <v>42</v>
+      </c>
+      <c r="H60">
+        <v>0.35</v>
+      </c>
+      <c r="I60">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>